<commit_message>
Final list of CMIP6 models (daily and monthly data)
DAILY (36 models) - precipitation (pr), temperature (tas, tasmin and tasmax).
MONTHLY (48 models) - wind (sfcWind) and snow (prsn). 
MONTHLY land (42 models): snow water equivalent (snw), snow cover (snc) and total soil moisture (mrso).
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Desktop/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47413018-7110-EE48-A433-25FB80DE672D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E903D09-FE02-754D-B935-B1293FD3BBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="1040" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
+    <workbookView xWindow="10920" yWindow="680" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="103">
   <si>
     <t>hist</t>
   </si>
@@ -1510,7 +1510,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2055,7 +2055,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -2067,16 +2067,28 @@
         <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="J15" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="K15" s="1">
-        <v>115.687261263</v>
+        <v>45.000454378999997</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>62</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2084,7 +2096,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -2098,7 +2110,7 @@
       <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -2107,17 +2119,14 @@
       <c r="I16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="4" t="s">
         <v>80</v>
       </c>
       <c r="K16" s="1">
-        <v>45.000454378999997</v>
+        <v>115.379159147</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2125,7 +2134,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2152,7 +2161,7 @@
         <v>80</v>
       </c>
       <c r="K17" s="1">
-        <v>115.379159147</v>
+        <v>115.73568678399999</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>62</v>
@@ -2163,19 +2172,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>80</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>80</v>
@@ -2190,7 +2199,7 @@
         <v>80</v>
       </c>
       <c r="K18" s="1">
-        <v>115.73568678399999</v>
+        <v>16.816434255000001</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>62</v>
@@ -2201,7 +2210,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -2228,7 +2237,7 @@
         <v>80</v>
       </c>
       <c r="K19" s="1">
-        <v>16.816434255000001</v>
+        <v>16.823844715</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>62</v>
@@ -2239,34 +2248,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K20" s="1">
-        <v>16.823844715</v>
+        <v>15.294436826</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>62</v>
@@ -2277,34 +2286,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="K21" s="1">
-        <v>15.294436826</v>
+        <v>31.092069240000001</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>62</v>
@@ -2315,31 +2321,34 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K22" s="1">
-        <v>31.092069240000001</v>
+        <v>6.1996430370000004</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>62</v>
@@ -2350,10 +2359,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -2377,7 +2386,7 @@
         <v>80</v>
       </c>
       <c r="K23" s="1">
-        <v>6.1996430370000004</v>
+        <v>23.192044070000001</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>62</v>
@@ -2388,10 +2397,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -2400,7 +2409,7 @@
         <v>80</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>80</v>
@@ -2408,14 +2417,11 @@
       <c r="H24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="J24" s="4" t="s">
         <v>80</v>
       </c>
       <c r="K24" s="1">
-        <v>23.192044070000001</v>
+        <v>18.964343237000001</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>62</v>
@@ -2426,10 +2432,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -2438,7 +2444,7 @@
         <v>80</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>80</v>
@@ -2446,11 +2452,14 @@
       <c r="H25" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="I25" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="J25" s="4" t="s">
         <v>80</v>
       </c>
       <c r="K25" s="1">
-        <v>18.964343237000001</v>
+        <v>18.986342571000002</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>62</v>
@@ -2461,10 +2470,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -2473,7 +2482,7 @@
         <v>80</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>80</v>
@@ -2488,7 +2497,7 @@
         <v>80</v>
       </c>
       <c r="K26" s="1">
-        <v>18.986342571000002</v>
+        <v>11.325136212</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>62</v>
@@ -2498,8 +2507,8 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>39</v>
+      <c r="B27" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -2526,18 +2535,21 @@
         <v>80</v>
       </c>
       <c r="K27" s="1">
-        <v>11.325136212</v>
+        <v>40.484891871999999</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>62</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>42</v>
+      <c r="B28" t="s">
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -2549,7 +2561,7 @@
         <v>80</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>80</v>
@@ -2564,13 +2576,10 @@
         <v>80</v>
       </c>
       <c r="K28" s="1">
-        <v>40.484891871999999</v>
+        <v>38.229036952000001</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2578,7 +2587,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -2586,37 +2595,34 @@
       <c r="D29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>80</v>
+      <c r="E29" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K29" s="1">
-        <v>38.229036952000001</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>62</v>
+        <v>32.788524181</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>41</v>
+      <c r="B30" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2631,27 +2637,27 @@
         <v>16</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K30" s="1">
-        <v>32.788524181</v>
+        <v>32.759743379</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>43</v>
+      <c r="B31" t="s">
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -2659,26 +2665,29 @@
       <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>92</v>
+      <c r="E31" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="K31" s="1">
-        <v>32.759743379</v>
+        <v>8.2013932080000007</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2686,7 +2695,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -2713,7 +2722,7 @@
         <v>80</v>
       </c>
       <c r="K32" s="1">
-        <v>8.2013932080000007</v>
+        <v>40.388901236000002</v>
       </c>
       <c r="L32" s="7" t="s">
         <v>62</v>
@@ -2724,34 +2733,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K33" s="1">
-        <v>40.388901236000002</v>
+        <v>19.008362587000001</v>
       </c>
       <c r="L33" s="7" t="s">
         <v>62</v>
@@ -2762,34 +2771,28 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>65</v>
+        <v>7</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>65</v>
+      <c r="H34" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="K34" s="1">
-        <v>19.008362587000001</v>
+        <v>38.472231819000001</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>62</v>
@@ -2800,7 +2803,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -2808,20 +2811,26 @@
       <c r="D35" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>94</v>
+      <c r="E35" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="K35" s="1">
-        <v>38.472231819000001</v>
+        <v>38.425875333</v>
       </c>
       <c r="L35" s="7" t="s">
         <v>62</v>
@@ -2832,34 +2841,31 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="K36" s="1">
-        <v>38.425875333</v>
+        <v>16.553534907</v>
       </c>
       <c r="L36" s="7" t="s">
         <v>62</v>
@@ -2870,34 +2876,31 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>65</v>
+      <c r="J37" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="K37" s="1">
-        <v>16.553534907</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>62</v>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2905,7 +2908,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>80</v>
@@ -2913,20 +2916,16 @@
       <c r="F38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="G38" s="6"/>
       <c r="H38" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I38" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="I38" s="6"/>
       <c r="J38" s="6" t="s">
         <v>80</v>
       </c>
       <c r="K38" s="1">
-        <v>40.799999999999997</v>
+        <v>115.73568678399999</v>
       </c>
       <c r="M38" s="17" t="s">
         <v>102</v>
@@ -2937,7 +2936,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>80</v>
@@ -2946,18 +2945,12 @@
         <v>16</v>
       </c>
       <c r="G39" s="6"/>
-      <c r="H39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6" t="s">
+      <c r="H39" s="6"/>
+      <c r="I39" s="6" t="s">
         <v>80</v>
       </c>
       <c r="K39" s="1">
-        <v>115.73568678399999</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>102</v>
+        <v>115.687261263</v>
       </c>
     </row>
     <row r="40" spans="1:13">

</xml_diff>

<commit_message>
Final list of CMIP6 models (daily and monthly data). Update
Change in model run: CESM2_r4i1p1f1
DAILY (36 models) - precipitation (pr), temperature (tas, tasmin and tasmax).
MONTHLY (48 models) - wind (sfcWind) and snow (prsn). 
MONTHLY land (42 models): snow water equivalent (snw), snow cover (snc) and total soil moisture (mrso).
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E903D09-FE02-754D-B935-B1293FD3BBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78075537-E552-A743-8F25-EDBFB25AAE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="680" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
+    <workbookView xWindow="6800" yWindow="680" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="104">
   <si>
     <t>hist</t>
   </si>
@@ -1044,6 +1044,9 @@
   </si>
   <si>
     <t>Daily data published after 30/11/2020</t>
+  </si>
+  <si>
+    <t>r4i1p1f1</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1513,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2625,7 +2628,7 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Final list of CMIP6 models (daily and monthly data). Errata CMCC-CM2-SR5
Tasmin and taxmax from CMCC-CM2-SR5.removed from the inventory. 
https://errata.es-doc.org/static/view.html?uid=33496f30-9e86-c0ff-874c-61f78df0509a

DAILY (36 models) - precipitation (pr), temperature (tas, tasmin and tasmax).
MONTHLY (48 models) - wind (sfcWind) and snow (prsn). 
MONTHLY land (42 models): snow water equivalent (snw), snow cover (snc) and total soil moisture (mrso).
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
+++ b/ATLAS-inventory/CMIP6_simulations_ATLAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78075537-E552-A743-8F25-EDBFB25AAE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34DDA1D-176B-984E-9E92-1B34E241A975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6800" yWindow="680" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="104">
   <si>
     <t>hist</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>CMCC.CMCC-ESM2</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <r>
@@ -1047,6 +1044,9 @@
   </si>
   <si>
     <t>r4i1p1f1</t>
+  </si>
+  <si>
+    <t>Problems with tasmin and tasmax ("X" dropped). https://errata.es-doc.org/static/view.html?uid=33496f30-9e86-c0ff-874c-61f78df0509a</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1513,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1582,22 +1582,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K2" s="1">
         <v>80.864219671000001</v>
@@ -1617,22 +1617,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1">
         <v>40.955032519</v>
@@ -1655,22 +1655,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="1">
         <v>61.678528151999998</v>
@@ -1693,22 +1693,22 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K5" s="1">
         <v>49.374977031999997</v>
@@ -1728,22 +1728,22 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K6" s="1">
         <v>17.579313868</v>
@@ -1766,22 +1766,22 @@
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K7" s="1">
         <v>8.1137502799999996</v>
@@ -1804,22 +1804,22 @@
         <v>3</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1">
         <v>10.117401146000001</v>
@@ -1839,28 +1839,28 @@
         <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="K9" s="1">
         <v>40.710173165999997</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>62</v>
+      <c r="M9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1877,28 +1877,25 @@
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K10" s="1">
         <v>172.948435115</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1915,22 +1912,22 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K11" s="1">
         <v>24.089237158</v>
@@ -1953,22 +1950,22 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K12" s="1">
         <v>24.079629625999999</v>
@@ -1991,22 +1988,22 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13" s="1">
         <v>24.253234431999999</v>
@@ -2029,22 +2026,22 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K14" s="1">
         <v>26.406662283999999</v>
@@ -2067,22 +2064,22 @@
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K15" s="1">
         <v>45.000454378999997</v>
@@ -2091,7 +2088,7 @@
         <v>62</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2108,22 +2105,22 @@
         <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K16" s="1">
         <v>115.379159147</v>
@@ -2146,22 +2143,22 @@
         <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K17" s="1">
         <v>115.73568678399999</v>
@@ -2184,22 +2181,22 @@
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="1">
         <v>16.816434255000001</v>
@@ -2222,22 +2219,22 @@
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19" s="1">
         <v>16.823844715</v>
@@ -2260,22 +2257,22 @@
         <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="G20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1">
         <v>15.294436826</v>
@@ -2298,19 +2295,19 @@
         <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" s="1">
         <v>31.092069240000001</v>
@@ -2333,22 +2330,22 @@
         <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K22" s="1">
         <v>6.1996430370000004</v>
@@ -2371,22 +2368,22 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K23" s="1">
         <v>23.192044070000001</v>
@@ -2409,19 +2406,19 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K24" s="1">
         <v>18.964343237000001</v>
@@ -2444,22 +2441,22 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K25" s="1">
         <v>18.986342571000002</v>
@@ -2482,22 +2479,22 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K26" s="1">
         <v>11.325136212</v>
@@ -2520,22 +2517,22 @@
         <v>3</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K27" s="1">
         <v>40.484891871999999</v>
@@ -2561,22 +2558,22 @@
         <v>3</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K28" s="1">
         <v>38.229036952000001</v>
@@ -2599,22 +2596,22 @@
         <v>3</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K29" s="1">
         <v>32.788524181</v>
@@ -2628,28 +2625,28 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K30" s="1">
         <v>32.759743379</v>
@@ -2669,22 +2666,22 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K31" s="1">
         <v>8.2013932080000007</v>
@@ -2707,22 +2704,22 @@
         <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K32" s="1">
         <v>40.388901236000002</v>
@@ -2745,22 +2742,22 @@
         <v>6</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K33" s="1">
         <v>19.008362587000001</v>
@@ -2783,16 +2780,16 @@
         <v>7</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K34" s="1">
         <v>38.472231819000001</v>
@@ -2815,22 +2812,22 @@
         <v>7</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="G35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K35" s="1">
         <v>38.425875333</v>
@@ -2853,19 +2850,19 @@
         <v>3</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K36" s="1">
         <v>16.553534907</v>
@@ -2882,28 +2879,28 @@
         <v>63</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K37" s="1">
         <v>40.799999999999997</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2911,27 +2908,27 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K38" s="1">
         <v>115.73568678399999</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2942,7 +2939,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>16</v>
@@ -2950,7 +2947,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K39" s="1">
         <v>115.687261263</v>
@@ -2964,22 +2961,22 @@
         <v>59</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M40" s="13"/>
     </row>
@@ -2991,22 +2988,22 @@
         <v>60</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M41" s="13"/>
     </row>
@@ -3015,10 +3012,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>16</v>
@@ -3027,7 +3024,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -3035,25 +3032,25 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -3061,25 +3058,25 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="1">
         <v>4.4000000000000004</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -3096,7 +3093,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>16</v>
@@ -3104,13 +3101,13 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K45" s="1">
         <v>11.195230902</v>
       </c>
       <c r="M45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -3118,25 +3115,25 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K46" s="1">
         <v>90.2</v>
       </c>
       <c r="M46" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -3144,29 +3141,29 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K47" s="1">
         <v>6.2</v>
       </c>
       <c r="M47" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -3174,21 +3171,21 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -3196,32 +3193,32 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="B51" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -3231,14 +3228,14 @@
     </row>
     <row r="53" spans="1:10">
       <c r="B53" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="12"/>
     </row>
     <row r="54" spans="1:10">
       <c r="B54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>